<commit_message>
EEPROM updates, preparing for config byte receiving from PC soft
</commit_message>
<xml_diff>
--- a/Interface_EEPROM.xlsx
+++ b/Interface_EEPROM.xlsx
@@ -18,9 +18,35 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
+  <si>
+    <t>FLOORID[1]</t>
+  </si>
+  <si>
+    <t>COUNT Data 1</t>
+  </si>
+  <si>
+    <t>COUNT Data 2</t>
+  </si>
+  <si>
+    <t>COUNT Data 3</t>
+  </si>
+  <si>
+    <t>FLOORID[2]</t>
+  </si>
+  <si>
+    <t>FLOORID[3]</t>
+  </si>
+  <si>
+    <t>FLOORID[4]</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +54,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -45,12 +89,60 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -331,12 +423,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="12" width="13.7109375" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" customWidth="1"/>
+    <col min="14" max="16" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>